<commit_message>
matrix de pesos final
</commit_message>
<xml_diff>
--- a/2021-02-03 - Analise de Exogeniedade Fraca.xlsx
+++ b/2021-02-03 - Analise de Exogeniedade Fraca.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bteba\Documents\GitHub\Tese\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A66D1D5-2B9C-4C61-97D1-81AC6D199BA6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D9CF2B-4C63-4C8A-A8C3-50D1B3B09181}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2021-02-03 - Ox_Results_Analise" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="19">
   <si>
     <t>region</t>
   </si>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>Exogeno fraco</t>
-  </si>
-  <si>
-    <t>PIB</t>
   </si>
   <si>
     <t>x</t>
@@ -995,7 +992,7 @@
   <dimension ref="A3:P555"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D571" sqref="D571"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1737,7 +1734,7 @@
         <v>Connection - 2020-11-13</v>
       </c>
     </row>
-    <row r="25" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>22</v>
       </c>
@@ -3694,8 +3691,8 @@
       <c r="A84">
         <v>81</v>
       </c>
-      <c r="B84" s="4" t="s">
-        <v>17</v>
+      <c r="B84" t="s">
+        <v>13</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>16</v>
@@ -3720,7 +3717,7 @@
       </c>
       <c r="K84" t="str">
         <f t="shared" si="1"/>
-        <v>PIB - 2020-12-14</v>
+        <v>Pib - 2020-12-14</v>
       </c>
     </row>
     <row r="85" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
@@ -10603,12 +10600,12 @@
         <v>Pib - 2020-11-30</v>
       </c>
     </row>
-    <row r="292" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="3">
         <v>289</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C292" s="3" t="s">
         <v>11</v>
@@ -10834,7 +10831,7 @@
         <v>Connection - 2020-11-13</v>
       </c>
     </row>
-    <row r="299" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>296</v>
       </c>
@@ -11626,12 +11623,12 @@
         <v>Connection - 2020-11-13</v>
       </c>
     </row>
-    <row r="323" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>320</v>
       </c>
       <c r="B323" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C323" t="s">
         <v>15</v>
@@ -16152,7 +16149,7 @@
       </c>
       <c r="O458" s="1"/>
     </row>
-    <row r="459" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A459">
         <v>456</v>
       </c>
@@ -16282,7 +16279,7 @@
       </c>
       <c r="P462" s="1"/>
     </row>
-    <row r="463" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A463">
         <v>460</v>
       </c>
@@ -19373,9 +19370,7 @@
   </sheetData>
   <autoFilter ref="A3:U555" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="1">
-      <filters>
-        <filter val="Equal Weight"/>
-      </filters>
+      <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -19402,7 +19397,7 @@
         <v>Connection - 2020-11-13</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="5:6" x14ac:dyDescent="0.25">
@@ -19410,7 +19405,7 @@
         <v>Pib per capta - 2020-11-30</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="5:6" x14ac:dyDescent="0.25">
@@ -19418,7 +19413,7 @@
         <v>Connection - 2020-12-14</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="5:6" x14ac:dyDescent="0.25">
@@ -19426,7 +19421,7 @@
         <v>Pib per capta - 2020-12-14</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="5:6" x14ac:dyDescent="0.25">
@@ -19439,7 +19434,7 @@
         <v>Pib - 2020-11-30</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="5:6" x14ac:dyDescent="0.25">
@@ -19447,15 +19442,15 @@
         <v>Populacao - 2020-11-30</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E11" t="str">
-        <v>PIB - 2020-12-14</v>
+        <v>Pib - 2020-12-14</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="5:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
log de exo fraca
</commit_message>
<xml_diff>
--- a/2021-02-03 - Analise de Exogeniedade Fraca.xlsx
+++ b/2021-02-03 - Analise de Exogeniedade Fraca.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bteba\Documents\GitHub\Tese\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D9CF2B-4C63-4C8A-A8C3-50D1B3B09181}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF425F16-F52B-4287-B872-AF85654BAE77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -992,7 +992,7 @@
   <dimension ref="A3:P555"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>